<commit_message>
added a decision tree regressor
</commit_message>
<xml_diff>
--- a/score.xlsx
+++ b/score.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://leeds365-my.sharepoint.com/personal/sc20dzi_leeds_ac_uk/Documents/Year 3/Semester 2/Individual Project/pain-detection-cats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{FE09CF12-BA22-E14D-ABFA-1BC09AB0AB4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D75AF07D-10CA-9444-9A8F-AA2011F8D218}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{FE09CF12-BA22-E14D-ABFA-1BC09AB0AB4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74852367-D84E-7B49-9919-DE6323BD715A}"/>
   <bookViews>
-    <workbookView xWindow="3860" yWindow="1940" windowWidth="26380" windowHeight="16440" xr2:uid="{0692187A-1C2E-4A48-BEDF-5E0FDA9AE14A}"/>
+    <workbookView xWindow="460" yWindow="700" windowWidth="26380" windowHeight="16440" xr2:uid="{0692187A-1C2E-4A48-BEDF-5E0FDA9AE14A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>method</t>
   </si>
@@ -51,13 +51,23 @@
   </si>
   <si>
     <t>logistic regression</t>
+  </si>
+  <si>
+    <t>decision tree regressor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -91,17 +101,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -413,15 +426,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F07C0E77-94EB-144C-8694-F1524DDF5FF0}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="3" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
@@ -440,10 +453,10 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="4">
         <v>0.22201281568036099</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <v>0.47118235926269703</v>
       </c>
     </row>
@@ -451,11 +464,22 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="4">
         <v>0.217866566151526</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <v>0.46676178737288099</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.22163588390501299</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.47078220432065299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added random forest regressor
</commit_message>
<xml_diff>
--- a/score.xlsx
+++ b/score.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://leeds365-my.sharepoint.com/personal/sc20dzi_leeds_ac_uk/Documents/Year 3/Semester 2/Individual Project/pain-detection-cats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{FE09CF12-BA22-E14D-ABFA-1BC09AB0AB4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74852367-D84E-7B49-9919-DE6323BD715A}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="8_{FE09CF12-BA22-E14D-ABFA-1BC09AB0AB4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC6A185C-4B85-8D4D-8130-D5AB977E476D}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="700" windowWidth="26380" windowHeight="16440" xr2:uid="{0692187A-1C2E-4A48-BEDF-5E0FDA9AE14A}"/>
+    <workbookView xWindow="420" yWindow="700" windowWidth="26380" windowHeight="16440" xr2:uid="{0692187A-1C2E-4A48-BEDF-5E0FDA9AE14A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>method</t>
   </si>
@@ -54,12 +54,24 @@
   </si>
   <si>
     <t>decision tree regressor</t>
+  </si>
+  <si>
+    <t>cross val mean</t>
+  </si>
+  <si>
+    <t>standard dev</t>
+  </si>
+  <si>
+    <t>random forest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -108,9 +120,9 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,60 +438,103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F07C0E77-94EB-144C-8694-F1524DDF5FF0}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="3" width="10.83203125" style="3"/>
+    <col min="4" max="4" width="16.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="2">
         <v>0.22201281568036099</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="2">
         <v>0.47118235926269703</v>
       </c>
+      <c r="D2" s="3">
+        <v>-0.16541844991079899</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2.02108777533173E-2</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="2">
         <v>0.217866566151526</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="2">
         <v>0.46676178737288099</v>
       </c>
+      <c r="D3" s="3">
+        <v>-0.22805646190949</v>
+      </c>
+      <c r="E3" s="3">
+        <v>2.1937123415589E-2</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="2">
         <v>0.22163588390501299</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="2">
         <v>0.47078220432065299</v>
+      </c>
+      <c r="D4" s="3">
+        <v>-0.16970438124085099</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2.2985981378926601E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.21409724839803901</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.46270643868228101</v>
+      </c>
+      <c r="D5" s="3">
+        <v>-0.16325451012216</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2.3304152509697602E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a neural network
</commit_message>
<xml_diff>
--- a/score.xlsx
+++ b/score.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://leeds365-my.sharepoint.com/personal/sc20dzi_leeds_ac_uk/Documents/Year 3/Semester 2/Individual Project/pain-detection-cats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="8_{FE09CF12-BA22-E14D-ABFA-1BC09AB0AB4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6DE4060-87C7-E143-8B11-F0B19DEA562B}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="8_{FE09CF12-BA22-E14D-ABFA-1BC09AB0AB4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E5CD2FE-498D-F24E-B027-D620D6DF486B}"/>
   <bookViews>
     <workbookView xWindow="420" yWindow="700" windowWidth="26380" windowHeight="16440" xr2:uid="{0692187A-1C2E-4A48-BEDF-5E0FDA9AE14A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>method</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>accuracy</t>
+  </si>
+  <si>
+    <t>NN (3 layers)</t>
   </si>
 </sst>
 </file>
@@ -444,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F07C0E77-94EB-144C-8694-F1524DDF5FF0}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -578,6 +581,14 @@
         <v>0.79645684131172201</v>
       </c>
     </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7">
+        <v>0.77647942304611195</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
wrote grid search for the neural network
</commit_message>
<xml_diff>
--- a/score.xlsx
+++ b/score.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://leeds365-my.sharepoint.com/personal/sc20dzi_leeds_ac_uk/Documents/Year 3/Semester 2/Individual Project/pain-detection-cats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="8_{FE09CF12-BA22-E14D-ABFA-1BC09AB0AB4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E5CD2FE-498D-F24E-B027-D620D6DF486B}"/>
+  <xr:revisionPtr revIDLastSave="103" documentId="8_{FE09CF12-BA22-E14D-ABFA-1BC09AB0AB4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7421D97-3868-9048-A3B0-B8ED31DE192D}"/>
   <bookViews>
     <workbookView xWindow="420" yWindow="700" windowWidth="26380" windowHeight="16440" xr2:uid="{0692187A-1C2E-4A48-BEDF-5E0FDA9AE14A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>method</t>
   </si>
@@ -71,7 +71,16 @@
     <t>accuracy</t>
   </si>
   <si>
-    <t>NN (3 layers)</t>
+    <t>NN (3 layers, 15 neurons)</t>
+  </si>
+  <si>
+    <t>best parameters</t>
+  </si>
+  <si>
+    <t>{'C': 10, 'gamma': 1, 'kernel': 'rbf'}</t>
+  </si>
+  <si>
+    <t>{'max_depth': 30, 'min_samples_leaf': 8, 'min_samples_split': 10, 'n_estimators': 200}</t>
   </si>
 </sst>
 </file>
@@ -105,12 +114,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -126,12 +141,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F07C0E77-94EB-144C-8694-F1524DDF5FF0}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -459,9 +476,10 @@
     <col min="2" max="3" width="10.83203125" style="3"/>
     <col min="4" max="4" width="16.33203125" style="3" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -477,11 +495,14 @@
       <c r="E1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -497,11 +518,11 @@
       <c r="E2" s="3">
         <v>2.02108777533173E-2</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="3">
         <v>0.78251036562382204</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -517,11 +538,11 @@
       <c r="E3" s="3">
         <v>2.1937123415589E-2</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>0.78665661515265695</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -537,31 +558,34 @@
       <c r="E4" s="3">
         <v>2.2985981378926601E-2</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>0.79532604598567602</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="6">
         <v>0.20768940821711199</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="6">
         <v>0.45572953406281702</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="6">
         <v>-0.15820166293882401</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="6">
         <v>2.1892703682266298E-2</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="6">
         <v>0.79947229551451104</v>
       </c>
+      <c r="G5" s="5" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -577,15 +601,18 @@
       <c r="E6" s="3">
         <v>2.3949357097771899E-2</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="3">
         <v>0.79645684131172201</v>
       </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <v>0.77647942304611195</v>
       </c>
     </row>

</xml_diff>